<commit_message>
added abstract and methods and adjusted personnel template
</commit_message>
<xml_diff>
--- a/chl-transect-underway-info.xlsx
+++ b/chl-transect-underway-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-chl-transect-underway-discrete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EADBDD-0290-416D-8C51-B000747D7D42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1855697D-E304-4801-AF70-77A042CCE29A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9756" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18060" windowHeight="9756" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personnel" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>attributeName</t>
   </si>
@@ -195,9 +195,6 @@
     <t>missing data</t>
   </si>
   <si>
-    <t>postdoctoral Researcher</t>
-  </si>
-  <si>
     <t>Organic matter</t>
   </si>
   <si>
@@ -207,9 +204,6 @@
     <t>Herbst</t>
   </si>
   <si>
-    <t>undergraduate Student</t>
-  </si>
-  <si>
     <t>preferred_fluorometer</t>
   </si>
   <si>
@@ -250,6 +244,21 @@
   </si>
   <si>
     <t>WETLabs WETStar fluorometer</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Futrelle</t>
+  </si>
+  <si>
+    <t>jfutrelle@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0003-4537-5853</t>
+  </si>
+  <si>
+    <t>softwareDeveloper</t>
   </si>
 </sst>
 </file>
@@ -631,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -707,22 +716,22 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>30</v>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -736,22 +745,22 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>55</v>
+      <c r="E4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -765,22 +774,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>68</v>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -815,14 +824,45 @@
         <v>14</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId4" xr:uid="{B1C88733-F7E0-42BD-8EAC-39DB55CA6A0F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -865,7 +905,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -921,7 +961,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>45</v>
@@ -929,7 +969,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>45</v>
@@ -953,7 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1005,7 +1045,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1016,7 +1056,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,46 +1083,46 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>61</v>
       </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>